<commit_message>
Updated Login Page test cases
</commit_message>
<xml_diff>
--- a/SauceDemoData.xlsx
+++ b/SauceDemoData.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>Test Case number</t>
   </si>
@@ -26,6 +26,12 @@
     <t>Password</t>
   </si>
   <si>
+    <t>standard_user</t>
+  </si>
+  <si>
+    <t>secret_sauce</t>
+  </si>
+  <si>
     <t>Attribute</t>
   </si>
   <si>
@@ -47,7 +53,16 @@
     <t>Password Placeholder</t>
   </si>
   <si>
-    <t>Passwor</t>
+    <t>Login Button Text</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Error Message</t>
+  </si>
+  <si>
+    <t>Epic sadface: Username is required</t>
   </si>
 </sst>
 </file>
@@ -55,13 +70,25 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -72,7 +99,14 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -84,10 +118,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -394,46 +437,62 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="2" width="27.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="2" width="35.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="5" width="27.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="35.71928571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
-      <c r="A1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
-      <c r="A2" s="1" t="s">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+      <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
-      <c r="A3" s="1" t="s">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+      <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
-      <c r="A4" s="1" t="s">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+      <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+      <c r="A4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+      <c r="A5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+      <c r="A6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -446,26 +505,37 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="2" width="21.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="2" width="25.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="2" width="27.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="4" width="21.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="25.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="5" width="27.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+      <c r="A2" s="3">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Test Plan in readme
</commit_message>
<xml_diff>
--- a/SauceDemoData.xlsx
+++ b/SauceDemoData.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>Test Case number</t>
   </si>
@@ -57,6 +57,12 @@
   </si>
   <si>
     <t>Login</t>
+  </si>
+  <si>
+    <t>Login Button Color</t>
+  </si>
+  <si>
+    <t>rgb(61, 220, 145)</t>
   </si>
   <si>
     <t>Error Message</t>
@@ -70,19 +76,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -118,16 +118,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -437,17 +434,17 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="27.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="35.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="4" width="27.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="4" width="35.71928571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -455,7 +452,7 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -463,7 +460,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -471,7 +468,7 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
@@ -479,7 +476,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
@@ -487,12 +484,20 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
       <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
+      <c r="A7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -511,9 +516,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="21.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="25.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="27.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="3" width="21.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="4" width="25.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="27.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -528,7 +533,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="3">
+      <c r="A2" s="1">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">

</xml_diff>